<commit_message>
New file and second floor
</commit_message>
<xml_diff>
--- a/map0.xlsx
+++ b/map0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arpit\coding\twiet\schoolSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067AF733-69D3-4270-892D-F5D23C4C1CAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D5BD82-8652-4061-A88F-C37972E0A590}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7185" yWindow="1035" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -407,8 +407,8 @@
   </sheetPr>
   <dimension ref="G1:CU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="BA48" sqref="BA48"/>
+    <sheetView tabSelected="1" topLeftCell="CO1" zoomScale="400" workbookViewId="0">
+      <selection activeCell="CV1" sqref="CV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>